<commit_message>
before sending to corrections
</commit_message>
<xml_diff>
--- a/11_spatial_join_example.xlsx
+++ b/11_spatial_join_example.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DS\mgr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE6C6EC0-0C48-4BE9-9259-15557BB487D0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80DE74F5-F4B9-4445-8BC7-812D450088C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -120,10 +120,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -407,7 +409,7 @@
   <dimension ref="B2:O15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="F19" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -469,7 +471,7 @@
       </c>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B5" s="1">
+      <c r="B5" s="3">
         <v>1</v>
       </c>
       <c r="C5" s="1">
@@ -640,7 +642,7 @@
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B14" s="2">
+      <c r="B14" s="4">
         <v>222</v>
       </c>
       <c r="C14" s="2">
@@ -657,5 +659,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>